<commit_message>
ref: adding labels to comparation tables in Excel
</commit_message>
<xml_diff>
--- a/Resumen de resultados.xlsx
+++ b/Resumen de resultados.xlsx
@@ -1,25 +1,115 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Universidad\Semestre 08\Bases de Datos II\Proyectos\BD2-T4\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{458B19DC-B338-4A08-9CCB-A83817A4D6B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Datos punto 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Datos punto 2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="23">
+  <si>
+    <t>Clientes</t>
+  </si>
+  <si>
+    <t>Facturas</t>
+  </si>
+  <si>
+    <t>Detalles</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>f+g</t>
+  </si>
+  <si>
+    <t>Tasa 1</t>
+  </si>
+  <si>
+    <t>Tasa 2</t>
+  </si>
+  <si>
+    <t>Tasa 3</t>
+  </si>
+  <si>
+    <t>Costos</t>
+  </si>
+  <si>
+    <t>Tiempos</t>
+  </si>
+  <si>
+    <t>Explain plan</t>
+  </si>
+  <si>
+    <t>TKPROF</t>
+  </si>
+  <si>
+    <t>Volumen de datos</t>
+  </si>
+  <si>
+    <t>CPU</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -49,8 +139,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +429,555 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AY4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="V4" sqref="V4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="7.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="51" width="3.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="52" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="2"/>
+      <c r="Z1" s="2"/>
+      <c r="AA1" s="2"/>
+      <c r="AB1" s="2"/>
+      <c r="AC1" s="2"/>
+      <c r="AD1" s="2"/>
+      <c r="AE1" s="2"/>
+      <c r="AF1" s="2"/>
+      <c r="AG1" s="2"/>
+      <c r="AH1" s="2"/>
+      <c r="AI1" s="2"/>
+      <c r="AJ1" s="2"/>
+      <c r="AK1" s="2"/>
+      <c r="AL1" s="2"/>
+      <c r="AM1" s="2"/>
+      <c r="AN1" s="2"/>
+      <c r="AO1" s="2"/>
+      <c r="AP1" s="2"/>
+      <c r="AQ1" s="2"/>
+      <c r="AR1" s="2"/>
+      <c r="AS1" s="2"/>
+      <c r="AT1" s="2"/>
+      <c r="AU1" s="2"/>
+      <c r="AV1" s="2"/>
+      <c r="AW1" s="2"/>
+      <c r="AX1" s="2"/>
+      <c r="AY1" s="2"/>
+    </row>
+    <row r="2" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y2" s="2"/>
+      <c r="Z2" s="2"/>
+      <c r="AA2" s="2"/>
+      <c r="AB2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="AC2" s="2"/>
+      <c r="AD2" s="2"/>
+      <c r="AE2" s="2"/>
+      <c r="AF2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG2" s="2"/>
+      <c r="AH2" s="2"/>
+      <c r="AI2" s="2"/>
+      <c r="AJ2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AK2" s="2"/>
+      <c r="AL2" s="2"/>
+      <c r="AM2" s="2"/>
+      <c r="AN2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="AO2" s="2"/>
+      <c r="AP2" s="2"/>
+      <c r="AQ2" s="2"/>
+      <c r="AR2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="AS2" s="2"/>
+      <c r="AT2" s="2"/>
+      <c r="AU2" s="2"/>
+      <c r="AV2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AW2" s="2"/>
+      <c r="AX2" s="2"/>
+      <c r="AY2" s="2"/>
+    </row>
+    <row r="3" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AD3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AE3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AF3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AG3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AH3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AI3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AJ3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AK3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AL3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AM3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AN3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AO3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AP3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AQ3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AR3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AS3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AT3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AU3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AV3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AW3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AX3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AY3" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>100</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1000</v>
+      </c>
+      <c r="C4" s="1">
+        <v>5000</v>
+      </c>
+      <c r="L4" s="1">
+        <f>AV4/AF4</f>
+        <v>6</v>
+      </c>
+      <c r="M4" s="1">
+        <f t="shared" ref="M4:O4" si="0">AW4/AG4</f>
+        <v>4</v>
+      </c>
+      <c r="N4" s="1">
+        <f>AX4/AH4</f>
+        <v>3.3333333333333335</v>
+      </c>
+      <c r="O4" s="1">
+        <f>AY4/AI4</f>
+        <v>3</v>
+      </c>
+      <c r="P4" s="1">
+        <f>AJ4/AN4</f>
+        <v>0.25</v>
+      </c>
+      <c r="Q4" s="1">
+        <f t="shared" ref="Q4:S4" si="1">AK4/AO4</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="R4" s="1">
+        <f t="shared" si="1"/>
+        <v>1.5</v>
+      </c>
+      <c r="S4" s="1">
+        <f>AM4/AQ4</f>
+        <v>4</v>
+      </c>
+      <c r="T4" s="1">
+        <f>AR4/AV4</f>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="U4" s="1">
+        <f>AS4/AW4</f>
+        <v>0.75</v>
+      </c>
+      <c r="V4" s="1">
+        <f t="shared" ref="U4:W4" si="2">AT4/AX4</f>
+        <v>0.7</v>
+      </c>
+      <c r="W4" s="1">
+        <f>AU4/AY4</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="X4" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y4" s="1">
+        <v>2</v>
+      </c>
+      <c r="Z4" s="1">
+        <v>3</v>
+      </c>
+      <c r="AA4" s="1">
+        <v>4</v>
+      </c>
+      <c r="AB4" s="1">
+        <v>5</v>
+      </c>
+      <c r="AC4" s="1">
+        <v>6</v>
+      </c>
+      <c r="AD4" s="1">
+        <v>7</v>
+      </c>
+      <c r="AE4" s="1">
+        <v>8</v>
+      </c>
+      <c r="AF4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG4" s="1">
+        <v>2</v>
+      </c>
+      <c r="AH4" s="1">
+        <v>3</v>
+      </c>
+      <c r="AI4" s="1">
+        <v>4</v>
+      </c>
+      <c r="AJ4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AK4" s="1">
+        <v>2</v>
+      </c>
+      <c r="AL4" s="1">
+        <v>3</v>
+      </c>
+      <c r="AM4" s="1">
+        <v>4</v>
+      </c>
+      <c r="AN4" s="1">
+        <v>4</v>
+      </c>
+      <c r="AO4" s="1">
+        <v>3</v>
+      </c>
+      <c r="AP4" s="1">
+        <v>2</v>
+      </c>
+      <c r="AQ4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AR4" s="1">
+        <v>5</v>
+      </c>
+      <c r="AS4" s="1">
+        <v>6</v>
+      </c>
+      <c r="AT4" s="1">
+        <v>7</v>
+      </c>
+      <c r="AU4" s="1">
+        <v>8</v>
+      </c>
+      <c r="AV4" s="1">
+        <f>X4+AB4</f>
+        <v>6</v>
+      </c>
+      <c r="AW4" s="1">
+        <f>Y4+AC4</f>
+        <v>8</v>
+      </c>
+      <c r="AX4" s="1">
+        <f t="shared" ref="AW4:AY4" si="3">Z4+AD4</f>
+        <v>10</v>
+      </c>
+      <c r="AY4" s="1">
+        <f>AA4+AE4</f>
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="15">
+    <mergeCell ref="L1:AY1"/>
+    <mergeCell ref="A1:C2"/>
+    <mergeCell ref="L2:O2"/>
+    <mergeCell ref="P2:S2"/>
+    <mergeCell ref="T2:W2"/>
+    <mergeCell ref="AV2:AY2"/>
+    <mergeCell ref="AR2:AU2"/>
+    <mergeCell ref="AN2:AQ2"/>
+    <mergeCell ref="AJ2:AM2"/>
+    <mergeCell ref="AF2:AI2"/>
+    <mergeCell ref="AB2:AE2"/>
+    <mergeCell ref="X2:AA2"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="D1:K1"/>
+    <mergeCell ref="H2:K2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0613F32F-E4BA-4F48-BA6A-4833B75597D5}">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="16384" width="11.5546875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="2"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="3"/>
+      <c r="B2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="3"/>
+      <c r="B3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="A1:A3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ref: first results first point
</commit_message>
<xml_diff>
--- a/Resumen de resultados.xlsx
+++ b/Resumen de resultados.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Universidad\Semestre 08\Bases de Datos II\Proyectos\BD2-T4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{458B19DC-B338-4A08-9CCB-A83817A4D6B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{158CA986-3C24-4EFB-84AC-B62D6286B6DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos punto 1" sheetId="1" r:id="rId1"/>
@@ -110,6 +110,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="173" formatCode="0.000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -139,7 +142,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -149,6 +152,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -433,7 +442,7 @@
   <dimension ref="A1:AY4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V4" sqref="V4"/>
+      <selection activeCell="R16" sqref="R16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -441,7 +450,26 @@
     <col min="1" max="1" width="7.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="51" width="3.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="3.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="3.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="3.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="19" width="3.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="4.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="3.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="4" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="31" width="3.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="32" max="33" width="5" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="35" width="3.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="36" max="37" width="5" style="1" bestFit="1" customWidth="1"/>
+    <col min="38" max="39" width="3.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="40" max="41" width="4" style="1" bestFit="1" customWidth="1"/>
+    <col min="42" max="47" width="3.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="48" max="49" width="4" style="1" bestFit="1" customWidth="1"/>
+    <col min="50" max="51" width="3.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="52" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
@@ -746,141 +774,117 @@
       <c r="C4" s="1">
         <v>5000</v>
       </c>
+      <c r="D4" s="1">
+        <v>13</v>
+      </c>
+      <c r="E4" s="1">
+        <v>13</v>
+      </c>
+      <c r="H4" s="4">
+        <v>1</v>
+      </c>
+      <c r="I4" s="1">
+        <v>1</v>
+      </c>
       <c r="L4" s="1">
         <f>AV4/AF4</f>
-        <v>6</v>
+        <v>7.2400000000000006E-2</v>
       </c>
       <c r="M4" s="1">
-        <f t="shared" ref="M4:O4" si="0">AW4/AG4</f>
-        <v>4</v>
-      </c>
-      <c r="N4" s="1">
+        <f t="shared" ref="M4" si="0">AW4/AG4</f>
+        <v>7.2400000000000006E-2</v>
+      </c>
+      <c r="N4" s="1" t="e">
         <f>AX4/AH4</f>
-        <v>3.3333333333333335</v>
-      </c>
-      <c r="O4" s="1">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O4" s="1" t="e">
         <f>AY4/AI4</f>
-        <v>3</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="P4" s="1">
         <f>AJ4/AN4</f>
-        <v>0.25</v>
+        <v>14.925373134328359</v>
       </c>
       <c r="Q4" s="1">
         <f t="shared" ref="Q4:S4" si="1">AK4/AO4</f>
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="R4" s="1">
+        <v>14.925373134328359</v>
+      </c>
+      <c r="R4" s="1" t="e">
         <f t="shared" si="1"/>
-        <v>1.5</v>
-      </c>
-      <c r="S4" s="1">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S4" s="1" t="e">
         <f>AM4/AQ4</f>
-        <v>4</v>
-      </c>
-      <c r="T4" s="1">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T4" s="4">
         <f>AR4/AV4</f>
-        <v>0.83333333333333337</v>
-      </c>
-      <c r="U4" s="1">
+        <v>0</v>
+      </c>
+      <c r="U4" s="5">
         <f>AS4/AW4</f>
-        <v>0.75</v>
-      </c>
-      <c r="V4" s="1">
+        <v>7.4585635359116026E-2</v>
+      </c>
+      <c r="V4" s="1" t="e">
         <f t="shared" ref="U4:W4" si="2">AT4/AX4</f>
-        <v>0.7</v>
-      </c>
-      <c r="W4" s="1">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W4" s="1" t="e">
         <f>AU4/AY4</f>
-        <v>0.66666666666666663</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="X4" s="1">
-        <v>1</v>
+        <v>362</v>
       </c>
       <c r="Y4" s="1">
-        <v>2</v>
-      </c>
-      <c r="Z4" s="1">
-        <v>3</v>
-      </c>
-      <c r="AA4" s="1">
-        <v>4</v>
+        <v>362</v>
       </c>
       <c r="AB4" s="1">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="AC4" s="1">
-        <v>6</v>
-      </c>
-      <c r="AD4" s="1">
-        <v>7</v>
-      </c>
-      <c r="AE4" s="1">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AF4" s="1">
-        <v>1</v>
+        <v>5000</v>
       </c>
       <c r="AG4" s="1">
-        <v>2</v>
-      </c>
-      <c r="AH4" s="1">
-        <v>3</v>
-      </c>
-      <c r="AI4" s="1">
-        <v>4</v>
+        <v>5000</v>
       </c>
       <c r="AJ4" s="1">
-        <v>1</v>
+        <v>5000</v>
       </c>
       <c r="AK4" s="1">
-        <v>2</v>
-      </c>
-      <c r="AL4" s="1">
-        <v>3</v>
-      </c>
-      <c r="AM4" s="1">
-        <v>4</v>
+        <v>5000</v>
       </c>
       <c r="AN4" s="1">
-        <v>4</v>
+        <v>335</v>
       </c>
       <c r="AO4" s="1">
-        <v>3</v>
-      </c>
-      <c r="AP4" s="1">
-        <v>2</v>
-      </c>
-      <c r="AQ4" s="1">
-        <v>1</v>
+        <v>335</v>
       </c>
       <c r="AR4" s="1">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="AS4" s="1">
-        <v>6</v>
-      </c>
-      <c r="AT4" s="1">
-        <v>7</v>
-      </c>
-      <c r="AU4" s="1">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="AV4" s="1">
         <f>X4+AB4</f>
-        <v>6</v>
+        <v>362</v>
       </c>
       <c r="AW4" s="1">
         <f>Y4+AC4</f>
-        <v>8</v>
+        <v>362</v>
       </c>
       <c r="AX4" s="1">
         <f t="shared" ref="AW4:AY4" si="3">Z4+AD4</f>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="AY4" s="1">
         <f>AA4+AE4</f>
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>